<commit_message>
fix bugs && added detail_id to table item
</commit_message>
<xml_diff>
--- a/Excel/Item.xlsx
+++ b/Excel/Item.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="12080"/>
+    <workbookView windowWidth="18350" windowHeight="6880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="201">
   <si>
     <t>ID</t>
   </si>
@@ -86,6 +86,9 @@
     <t>贴图</t>
   </si>
   <si>
+    <t>详情id</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -110,6 +113,9 @@
     <t>png</t>
   </si>
   <si>
+    <t>detail_id</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
@@ -290,6 +296,9 @@
     <t>Item_200101</t>
   </si>
   <si>
+    <t>1011</t>
+  </si>
+  <si>
     <t>200102</t>
   </si>
   <si>
@@ -315,6 +324,9 @@
   </si>
   <si>
     <t>Item_200103</t>
+  </si>
+  <si>
+    <t>1031</t>
   </si>
   <si>
     <t>200104</t>
@@ -1391,7 +1403,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1417,6 +1429,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1737,13 +1752,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="9" style="10"/>
     <col min="2" max="2" width="19.125" style="10" customWidth="1"/>
@@ -1752,7 +1767,7 @@
     <col min="9" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" ht="26" customHeight="1" spans="1:8">
+    <row r="1" customFormat="1" ht="26" customHeight="1" spans="1:9">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1777,994 +1792,1043 @@
       <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="1" spans="1:8">
+      <c r="I1" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" spans="1:9">
       <c r="A2" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" customFormat="1" spans="1:8">
+        <v>16</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:9">
       <c r="A3" s="12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" customFormat="1" spans="1:8">
+        <v>19</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" spans="1:9">
       <c r="A4" s="10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" customFormat="1" spans="1:9">
+      <c r="A5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" customFormat="1" spans="1:8">
-      <c r="A5" s="10" t="s">
+      <c r="E5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" customFormat="1" spans="1:9">
+      <c r="A6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" customFormat="1" spans="1:9">
+      <c r="A7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" customFormat="1" spans="1:9">
+      <c r="A8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" customFormat="1" spans="1:9">
+      <c r="A9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" customFormat="1" spans="1:9">
+      <c r="A10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" customFormat="1" spans="1:9">
+      <c r="A11" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" customFormat="1" spans="1:9">
+      <c r="A12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" s="10" customFormat="1" spans="1:9">
+      <c r="A13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="E13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" customFormat="1" spans="1:8">
-      <c r="A6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" customFormat="1" spans="1:8">
-      <c r="A7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" customFormat="1" spans="1:8">
-      <c r="A8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" customFormat="1" spans="1:8">
-      <c r="A9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" customFormat="1" spans="1:8">
-      <c r="A10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" customFormat="1" spans="1:8">
-      <c r="A11" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" customFormat="1" spans="1:8">
-      <c r="A12" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" s="10" customFormat="1" spans="1:8">
-      <c r="A13" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="G13" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="14" s="10" customFormat="1" spans="1:8">
       <c r="A14" s="10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" s="10" customFormat="1" spans="1:8">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" s="10" customFormat="1" spans="1:9">
       <c r="A15" s="10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="16" s="10" customFormat="1" spans="1:8">
       <c r="A16" s="10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" s="10" customFormat="1" spans="1:8">
       <c r="A17" s="10" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="G17" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" s="10" customFormat="1" spans="1:8">
       <c r="A18" s="10" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" customFormat="1" spans="1:9">
+      <c r="A19" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" customFormat="1" spans="1:9">
+      <c r="A20" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" customFormat="1" spans="1:9">
+      <c r="A21" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" customFormat="1" spans="1:9">
+      <c r="A22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" customFormat="1" spans="1:9">
+      <c r="A23" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" customFormat="1" spans="1:9">
+      <c r="A24" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" customFormat="1" spans="1:9">
+      <c r="A25" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" customFormat="1" spans="1:9">
+      <c r="A26" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" customFormat="1" spans="1:9">
+      <c r="A27" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" customFormat="1" spans="1:9">
+      <c r="A28" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" s="14">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="29" customFormat="1" spans="1:9">
+      <c r="A29" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" s="14">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="30" customFormat="1" spans="1:9">
+      <c r="A30" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="I30" s="14"/>
+    </row>
+    <row r="31" customFormat="1" spans="1:9">
+      <c r="A31" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32" customFormat="1" spans="1:9">
+      <c r="A32" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="I32" s="14"/>
+    </row>
+    <row r="33" customFormat="1" spans="1:9">
+      <c r="A33" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="I33" s="14"/>
+    </row>
+    <row r="34" customFormat="1" spans="1:9">
+      <c r="A34" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" customFormat="1" spans="1:8">
-      <c r="A19" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="E34" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" customFormat="1" spans="1:8">
-      <c r="A20" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="H34" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="I34" s="14"/>
+    </row>
+    <row r="35" customFormat="1" spans="1:9">
+      <c r="A35" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" customFormat="1" spans="1:8">
-      <c r="A21" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="E35" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="I35" s="14"/>
+    </row>
+    <row r="36" customFormat="1" spans="1:9">
+      <c r="A36" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" customFormat="1" spans="1:8">
-      <c r="A22" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="E36" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="I36" s="14"/>
+    </row>
+    <row r="37" customFormat="1" spans="1:9">
+      <c r="A37" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" customFormat="1" spans="1:8">
-      <c r="A23" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="E37" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="I37" s="14"/>
+    </row>
+    <row r="38" customFormat="1" spans="1:9">
+      <c r="A38" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" customFormat="1" spans="1:8">
-      <c r="A24" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="E38" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="I38" s="14"/>
+    </row>
+    <row r="39" customFormat="1" spans="1:9">
+      <c r="A39" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" customFormat="1" spans="1:8">
-      <c r="A25" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="11" t="s">
+      <c r="E39" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" customFormat="1" spans="1:8">
-      <c r="A26" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" customFormat="1" spans="1:8">
-      <c r="A27" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" customFormat="1" spans="1:8">
-      <c r="A28" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" customFormat="1" spans="1:8">
-      <c r="A29" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" customFormat="1" spans="1:8">
-      <c r="A30" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" customFormat="1" spans="1:8">
-      <c r="A31" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" customFormat="1" spans="1:8">
-      <c r="A32" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" customFormat="1" spans="1:8">
-      <c r="A33" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" customFormat="1" spans="1:8">
-      <c r="A34" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="35" customFormat="1" spans="1:8">
-      <c r="A35" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" customFormat="1" spans="1:8">
-      <c r="A36" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="37" customFormat="1" spans="1:8">
-      <c r="A37" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="38" customFormat="1" spans="1:8">
-      <c r="A38" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="39" customFormat="1" spans="1:8">
-      <c r="A39" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>121</v>
-      </c>
       <c r="F39" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>188</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="I39" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2792,17 +2856,17 @@
     <row r="1" ht="16.5" spans="1:3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" ht="16.5" spans="1:3">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" ht="16.5" spans="1:3">
@@ -2817,10 +2881,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" ht="16.5" spans="1:3">
@@ -2828,10 +2892,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" ht="16.5" spans="1:3">
@@ -2839,7 +2903,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C6" s="8"/>
     </row>

</xml_diff>